<commit_message>
Updated User Manual as pdf
</commit_message>
<xml_diff>
--- a/Inputs/DailyTradingPlan.xlsx
+++ b/Inputs/DailyTradingPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\Momentum-Trading-Assistant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB12CC-C92C-4781-A479-F58A620C2F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931A623-4AE0-40DA-911D-9A4C296985CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Symbol</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t>NASDAQ</t>
-  </si>
-  <si>
-    <t>NVDA</t>
   </si>
   <si>
     <t>NYSE</t>
@@ -670,7 +667,7 @@
   <dimension ref="A1:CA290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,7 +961,7 @@
         <v>70</v>
       </c>
       <c r="BT1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BU1" t="s">
         <v>71</v>
@@ -1028,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
         <v>78</v>
@@ -1036,26 +1033,26 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>83</v>
       </c>
       <c r="H3" s="1">
-        <v>117.2</v>
+        <v>36</v>
       </c>
       <c r="I3" s="1">
-        <v>113</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="K3">
-        <v>118.37</v>
+        <v>37.5</v>
       </c>
       <c r="L3">
-        <v>140.63999999999999</v>
+        <v>54.1</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -1066,7 +1063,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
         <v>78</v>
@@ -1078,25 +1075,22 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="1">
-        <v>160.47</v>
+        <v>153</v>
       </c>
       <c r="I4" s="1">
-        <v>158.35</v>
+        <v>135</v>
       </c>
       <c r="J4" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="K4">
-        <v>161.66999999999999</v>
+        <v>155</v>
       </c>
       <c r="L4">
         <v>176.52</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:79" x14ac:dyDescent="0.3">
@@ -1104,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
         <v>78</v>
@@ -1119,16 +1113,16 @@
         <v>83</v>
       </c>
       <c r="H5" s="1">
-        <v>45.08</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1">
-        <v>45.08</v>
+        <v>30</v>
       </c>
       <c r="J5" s="2">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="K5">
-        <v>45.42</v>
+        <v>37.5</v>
       </c>
       <c r="L5">
         <v>54.1</v>

</xml_diff>

<commit_message>
Improved path-handling through new function get_directory_path() and debugged dailytradingplan_stop_update()
</commit_message>
<xml_diff>
--- a/Inputs/DailyTradingPlan.xlsx
+++ b/Inputs/DailyTradingPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\Momentum-Trading-Assistant\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931A623-4AE0-40DA-911D-9A4C296985CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423C0028-6406-4086-8364-A84B6891B577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -39,6 +36,12 @@
     <t>Symbol</t>
   </si>
   <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Security Type</t>
+  </si>
+  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -63,241 +66,235 @@
     <t>Profit taker price [$]</t>
   </si>
   <si>
+    <t>Open position</t>
+  </si>
+  <si>
+    <t>Add and reduce</t>
+  </si>
+  <si>
+    <t>Sell on close</t>
+  </si>
+  <si>
+    <t>Stop low of day</t>
+  </si>
+  <si>
+    <t>Sell bellow SMA [$]</t>
+  </si>
+  <si>
+    <t>Stop undercut [time]</t>
+  </si>
+  <si>
+    <t>Stop undercut</t>
+  </si>
+  <si>
+    <t>Crossed buy price [time]</t>
+  </si>
+  <si>
+    <t>Crossed buy price</t>
+  </si>
+  <si>
+    <t>Order executed [time]</t>
+  </si>
+  <si>
+    <t>Order executed</t>
+  </si>
+  <si>
+    <t>parentOrderId</t>
+  </si>
+  <si>
+    <t>Order filled</t>
+  </si>
+  <si>
+    <t>profitOrderId</t>
+  </si>
+  <si>
+    <t>Profit order filled</t>
+  </si>
+  <si>
+    <t>stopOrderId</t>
+  </si>
+  <si>
+    <t>Stop order filled</t>
+  </si>
+  <si>
+    <t>sellOnCloseOrderId</t>
+  </si>
+  <si>
+    <t>SOC order filled</t>
+  </si>
+  <si>
+    <t>Spread at execution [%]</t>
+  </si>
+  <si>
+    <t>2% above buy point</t>
+  </si>
+  <si>
+    <t>New OCA bracket [time]</t>
+  </si>
+  <si>
+    <t>New OCA bracket</t>
+  </si>
+  <si>
+    <t>5% above buy point [time]</t>
+  </si>
+  <si>
+    <t>5% above buy point</t>
+  </si>
+  <si>
+    <t>Bad close rule [time]</t>
+  </si>
+  <si>
+    <t>Bad close rule</t>
+  </si>
+  <si>
+    <t>Stock sold [time]</t>
+  </si>
+  <si>
+    <t>Stock sold</t>
+  </si>
+  <si>
+    <t>Spread above limit</t>
+  </si>
+  <si>
+    <t>Price above limit</t>
+  </si>
+  <si>
+    <t>Stock looped</t>
+  </si>
+  <si>
+    <t>Open position bracket submitted</t>
+  </si>
+  <si>
+    <t>Add and reduce executed</t>
+  </si>
+  <si>
+    <t>Open position updated</t>
+  </si>
+  <si>
+    <t>Open position updated [time]</t>
+  </si>
+  <si>
+    <t>New position updated</t>
+  </si>
+  <si>
+    <t>New position updated [time]</t>
+  </si>
+  <si>
+    <t>New position added</t>
+  </si>
+  <si>
+    <t>New position added [time]</t>
+  </si>
+  <si>
+    <t>Stop timestamp</t>
+  </si>
+  <si>
+    <t>Last stop price</t>
+  </si>
+  <si>
+    <t>Invest limit reached [time]</t>
+  </si>
+  <si>
+    <t>Invest limit reached</t>
+  </si>
+  <si>
+    <t>Position below limit</t>
+  </si>
+  <si>
+    <t>Max. daily loss reached [time]</t>
+  </si>
+  <si>
+    <t>Max. daily loss reached</t>
+  </si>
+  <si>
+    <t>LAST price [$]</t>
+  </si>
+  <si>
+    <t>BID price [$]</t>
+  </si>
+  <si>
+    <t>ASK price [$]</t>
+  </si>
+  <si>
+    <t>BID size</t>
+  </si>
+  <si>
+    <t>ASK size</t>
+  </si>
+  <si>
+    <t>HIGH price [$]</t>
+  </si>
+  <si>
+    <t>LOW price [$]</t>
+  </si>
+  <si>
+    <t>CLOSE price [$]</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>MAX_STOCK_SPREAD</t>
+  </si>
+  <si>
+    <t>SELL_HALF_REVERSAL_RULE</t>
+  </si>
+  <si>
+    <t>SELL_FULL_REVERSAL_RULE</t>
+  </si>
+  <si>
+    <t>BAD_CLOSE_RULE</t>
+  </si>
+  <si>
+    <t>MAX_ALLOWED_DAILY_PNL_LOSS</t>
+  </si>
+  <si>
+    <t>MIN_POSITION_SIZE</t>
+  </si>
+  <si>
+    <t>Bad close checked</t>
+  </si>
+  <si>
+    <t>liquidHours</t>
+  </si>
+  <si>
+    <t>timeZoneId</t>
+  </si>
+  <si>
+    <t>local opening time</t>
+  </si>
+  <si>
+    <t>local closing time</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>CRYPTO</t>
+  </si>
+  <si>
     <t>USD</t>
   </si>
   <si>
     <t>SMART</t>
   </si>
   <si>
-    <t>Security Type</t>
-  </si>
-  <si>
-    <t>Company name</t>
-  </si>
-  <si>
-    <t>BID size</t>
-  </si>
-  <si>
-    <t>ASK size</t>
-  </si>
-  <si>
-    <t>Stop undercut</t>
-  </si>
-  <si>
-    <t>LAST price [$]</t>
-  </si>
-  <si>
-    <t>BID price [$]</t>
-  </si>
-  <si>
-    <t>ASK price [$]</t>
-  </si>
-  <si>
-    <t>CLOSE price [$]</t>
-  </si>
-  <si>
-    <t>Spread at execution [%]</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>parentOrderId</t>
-  </si>
-  <si>
-    <t>Crossed buy price</t>
-  </si>
-  <si>
-    <t>Stop undercut [time]</t>
-  </si>
-  <si>
-    <t>Crossed buy price [time]</t>
-  </si>
-  <si>
-    <t>2% above buy point</t>
-  </si>
-  <si>
-    <t>5% above buy point</t>
-  </si>
-  <si>
-    <t>Stock sold</t>
-  </si>
-  <si>
-    <t>Order filled</t>
-  </si>
-  <si>
-    <t>New OCA bracket</t>
-  </si>
-  <si>
-    <t>Order executed</t>
-  </si>
-  <si>
-    <t>Open position</t>
-  </si>
-  <si>
-    <t>Stop timestamp</t>
-  </si>
-  <si>
-    <t>Open position bracket submitted</t>
-  </si>
-  <si>
-    <t>Last stop price</t>
-  </si>
-  <si>
-    <t>Order executed [time]</t>
-  </si>
-  <si>
-    <t>5% above buy point [time]</t>
-  </si>
-  <si>
-    <t>New OCA bracket [time]</t>
-  </si>
-  <si>
-    <t>Stock sold [time]</t>
-  </si>
-  <si>
-    <t>Invest limit reached</t>
-  </si>
-  <si>
-    <t>Max. daily loss reached</t>
-  </si>
-  <si>
-    <t>Invest limit reached [time]</t>
-  </si>
-  <si>
-    <t>Max. daily loss reached [time]</t>
-  </si>
-  <si>
-    <t>Add and reduce</t>
-  </si>
-  <si>
-    <t>Add and reduce executed</t>
-  </si>
-  <si>
-    <t>profitOrderId</t>
-  </si>
-  <si>
-    <t>Profit order filled</t>
-  </si>
-  <si>
-    <t>stopOrderId</t>
-  </si>
-  <si>
-    <t>Stop order filled</t>
-  </si>
-  <si>
-    <t>Sell on close</t>
-  </si>
-  <si>
-    <t>Sell bellow SMA [$]</t>
-  </si>
-  <si>
-    <t>Position below limit</t>
-  </si>
-  <si>
-    <t>sellOnCloseOrderId</t>
-  </si>
-  <si>
-    <t>SOC order filled</t>
-  </si>
-  <si>
-    <t>Spread above limit</t>
-  </si>
-  <si>
-    <t>Price above limit</t>
-  </si>
-  <si>
-    <t>Stock looped</t>
-  </si>
-  <si>
-    <t>Open position updated</t>
-  </si>
-  <si>
-    <t>Open position updated [time]</t>
-  </si>
-  <si>
-    <t>New position updated</t>
-  </si>
-  <si>
-    <t>New position updated [time]</t>
-  </si>
-  <si>
-    <t>New position added</t>
-  </si>
-  <si>
-    <t>New position added [time]</t>
-  </si>
-  <si>
-    <t>HIGH price [$]</t>
-  </si>
-  <si>
-    <t>LOW price [$]</t>
-  </si>
-  <si>
-    <t>Bad close rule</t>
-  </si>
-  <si>
-    <t>Bad close rule [time]</t>
-  </si>
-  <si>
-    <t>MAX_STOCK_SPREAD</t>
-  </si>
-  <si>
-    <t>SELL_HALF_REVERSAL_RULE</t>
-  </si>
-  <si>
-    <t>SELL_FULL_REVERSAL_RULE</t>
-  </si>
-  <si>
-    <t>MAX_ALLOWED_DAILY_PNL_LOSS</t>
-  </si>
-  <si>
-    <t>MIN_POSITION_SIZE</t>
-  </si>
-  <si>
-    <t>Bad close checked</t>
-  </si>
-  <si>
-    <t>liquidHours</t>
-  </si>
-  <si>
-    <t>timeZoneId</t>
-  </si>
-  <si>
-    <t>local opening time</t>
-  </si>
-  <si>
-    <t>local closing time</t>
+    <t>PAXOS</t>
+  </si>
+  <si>
+    <t>HROW</t>
   </si>
   <si>
     <t>STK</t>
   </si>
   <si>
-    <t>BTC</t>
-  </si>
-  <si>
-    <t>CRYPTO</t>
-  </si>
-  <si>
-    <t>PAXOS</t>
-  </si>
-  <si>
-    <t>Stop low of day</t>
-  </si>
-  <si>
     <t>NASDAQ</t>
   </si>
   <si>
+    <t>LDOS</t>
+  </si>
+  <si>
     <t>NYSE</t>
-  </si>
-  <si>
-    <t>LDOS</t>
-  </si>
-  <si>
-    <t>HROW</t>
-  </si>
-  <si>
-    <t>BAD_CLOSE_RULE</t>
   </si>
 </sst>
 </file>
@@ -350,7 +347,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="List Panel Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="List Panel Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -667,7 +664,7 @@
   <dimension ref="A1:CA290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,214 +751,214 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="U1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="V1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="X1" t="s">
         <v>22</v>
       </c>
       <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AZ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="BE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>35</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>18</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>70</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>87</v>
       </c>
       <c r="BU1" t="s">
         <v>71</v>
@@ -990,19 +987,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>80</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H2" s="1">
         <v>9</v>
@@ -1025,19 +1022,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H3" s="1">
         <v>36</v>
@@ -1063,19 +1060,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H4" s="1">
         <v>153</v>
@@ -1098,19 +1095,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H5" s="1">
         <v>36</v>
@@ -2565,6 +2562,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the possibility to limit the maximum absolute risk to be taken during the trading day. Added "Quantity [#] at open" to DailyTradingPlan.xlsx.
</commit_message>
<xml_diff>
--- a/Inputs/DailyTradingPlan.xlsx
+++ b/Inputs/DailyTradingPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\ibbot-python311\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\Momentum-Trading-Assistant\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6390BD-AA04-4F40-889C-DD799B116F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642473DC-BCFB-4C6D-B1D9-A9B1F573634F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
   <si>
     <t>Symbol</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>x-R profits</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>Quantity [#] at open</t>
   </si>
 </sst>
 </file>
@@ -682,10 +691,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:CI290"/>
+  <dimension ref="A1:CJ290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,56 +733,57 @@
     <col min="34" max="34" width="13.77734375" customWidth="1"/>
     <col min="35" max="36" width="17.88671875" customWidth="1"/>
     <col min="37" max="37" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="17.44140625" customWidth="1"/>
-    <col min="46" max="46" width="16" customWidth="1"/>
-    <col min="47" max="47" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.88671875" customWidth="1"/>
-    <col min="51" max="51" width="13" customWidth="1"/>
-    <col min="52" max="52" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.33203125" customWidth="1"/>
-    <col min="55" max="55" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="26.5546875" customWidth="1"/>
-    <col min="60" max="60" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="23" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="17.88671875" customWidth="1"/>
-    <col min="65" max="65" width="27" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="24.77734375" customWidth="1"/>
-    <col min="67" max="67" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="12.33203125" customWidth="1"/>
-    <col min="74" max="74" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="16" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.21875" customWidth="1"/>
-    <col min="85" max="85" width="11.21875" customWidth="1"/>
-    <col min="86" max="86" width="16" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.77734375" customWidth="1"/>
+    <col min="39" max="39" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="17.44140625" customWidth="1"/>
+    <col min="47" max="47" width="16" customWidth="1"/>
+    <col min="48" max="48" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.88671875" customWidth="1"/>
+    <col min="52" max="52" width="13" customWidth="1"/>
+    <col min="53" max="53" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.33203125" customWidth="1"/>
+    <col min="56" max="56" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="26.5546875" customWidth="1"/>
+    <col min="61" max="61" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="23" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.88671875" customWidth="1"/>
+    <col min="66" max="66" width="27" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.77734375" customWidth="1"/>
+    <col min="68" max="68" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="12.33203125" customWidth="1"/>
+    <col min="75" max="75" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="16" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="13.21875" customWidth="1"/>
+    <col min="86" max="86" width="11.21875" customWidth="1"/>
+    <col min="87" max="87" width="16" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -883,157 +893,160 @@
         <v>20</v>
       </c>
       <c r="AL1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM1" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>67</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>66</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>92</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>93</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>39</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>28</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>55</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>56</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>57</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>34</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>45</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>33</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>35</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>42</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>40</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>52</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>43</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>41</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>16</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>17</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>18</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>13</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>14</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>64</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>65</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>19</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>21</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>68</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>69</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>70</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>83</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>71</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>72</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>73</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>85</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>74</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>75</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>76</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1068,7 +1081,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1091,10 +1104,10 @@
         <v>54.95</v>
       </c>
       <c r="I3" s="1">
-        <v>61.4</v>
+        <v>44</v>
       </c>
       <c r="J3" s="2">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="K3">
         <v>55.5</v>
@@ -1118,79 +1131,203 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.3">
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.3">
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.3">
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="1">
+        <v>176</v>
+      </c>
+      <c r="I4" s="1">
+        <f>H4-10</f>
+        <v>166</v>
+      </c>
+      <c r="J4" s="2">
+        <v>100</v>
+      </c>
+      <c r="K4" s="1">
+        <v>185</v>
+      </c>
+      <c r="L4" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:88" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="1">
+        <v>176</v>
+      </c>
+      <c r="I5" s="1">
+        <f>H5-10</f>
+        <v>166</v>
+      </c>
+      <c r="J5" s="2">
+        <v>100</v>
+      </c>
+      <c r="K5" s="1">
+        <v>179</v>
+      </c>
+      <c r="L5" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:88" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="1">
+        <v>476</v>
+      </c>
+      <c r="I6" s="1">
+        <f>H6-10</f>
+        <v>466</v>
+      </c>
+      <c r="J6" s="2">
+        <v>100</v>
+      </c>
+      <c r="K6" s="1">
+        <f>H6+7</f>
+        <v>483</v>
+      </c>
+      <c r="L6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:88" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="1">
+        <v>476</v>
+      </c>
+      <c r="I7" s="1">
+        <f>H7-10</f>
+        <v>466</v>
+      </c>
+      <c r="J7" s="2">
+        <v>100</v>
+      </c>
+      <c r="K7" s="1">
+        <f>H7+7</f>
+        <v>483</v>
+      </c>
+      <c r="L7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:88" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.3">
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.3">
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.3">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.3">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.3">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>

</xml_diff>